<commit_message>
Editorial changes in release_notes.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/doc/evolution/Annotations Proposal/ESPD-CriteriaTaxonomy-SELFCONTAINED-V2.0.3-Annotated-Proposal.xlsx
+++ b/docs/src/main/asciidoc/dist/doc/evolution/Annotations Proposal/ESPD-CriteriaTaxonomy-SELFCONTAINED-V2.0.3-Annotated-Proposal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estaromi\OneDrive - everis\Projects\GROW\ESPD-EDM-v2.0.3\Annotated Method Proposal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESPDv2.1.0\docs\src\main\asciidoc\dist\doc\evolution\Annotations Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12833"/>
   </bookViews>
   <sheets>
     <sheet name="SC-Suitability-I" sheetId="10" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -39,9 +39,6 @@
     <t>ElementUUID</t>
   </si>
   <si>
-    <t>Element Code</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -165,12 +162,6 @@
     <t>6ee55a59-6adb-4c3a-b89f-e62a7ad7be7f</t>
   </si>
   <si>
-    <t>CRITERION.SELECTION.SUITABILITY.PROFESSIONAL_REGISTER_ENROLMENT</t>
-  </si>
-  <si>
-    <t>REGULATED_SC-Suitability_DS</t>
-  </si>
-  <si>
     <t>[Capton]</t>
   </si>
   <si>
@@ -253,92 +244,73 @@
   </si>
   <si>
     <t>CRITERION_REQUIREMENT_GROUP</t>
+  </si>
+  <si>
+    <t>CRITERION_QUESTION_SUBGROUP</t>
+  </si>
+  <si>
+    <t>CRITERION_REQUIREMENT_SUBGROUP</t>
+  </si>
+  <si>
+    <t>@espd:dataStructureType</t>
+  </si>
+  <si>
+    <t>EVIDENCE</t>
+  </si>
+  <si>
+    <t>Annotations (marked as @[AnnotationXXXXX] would be subclasses of Processing Instructions used by software processors to know how to process an element (in this case a data element). Thus annotations can be used to warn a processor reading a criterion about the type of data structure, so the processor knows what algorithms to apply to this particular instance of data structure. See for example the annotation about the Evidence data structure, at the end of this example</t>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
+        <color theme="1" tint="0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>In a future version 3.0.0</t>
+      <t>In future versions</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
+        <color theme="1" tint="0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>,</t>
+      <t>,  the codes ON*, ONTRUE and ONFALSE used to process or not blocks of requirements and questions depending on the response given to the most previous Indicator would be specified by means of the annotation property @espd:groupVisibilityDependencyType (as shown below)</t>
     </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
+        <color theme="1" tint="0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> the </t>
+      <t xml:space="preserve">In future versions, the </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
+        <color theme="1" tint="0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>CriterionPropertyGroupType element will hold one of the following code values: CRITERION_REQUIREMENT_GROUP, CRITERION_REQUIREMENT_SUBGROUP, CRITERION_QUESTION_GROUP, CRITERION_QUESTION_SUBGROUP (instead of ON*, ONTRUE and ONFALSE)</t>
+      <t>CriterionPropertyGroupType element would hold one of the following code values: CRITERION_REQUIREMENT_GROUP, CRITERION_REQUIREMENT_SUBGROUP, CRITERION_QUESTION_GROUP, CRITERION_QUESTION_SUBGROUP (instead of ON*, ONTRUE and ONFALSE)</t>
     </r>
   </si>
   <si>
-    <t>CRITERION_QUESTION_SUBGROUP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>In a future version 3.0.0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>,  the codes ON*, ONTRUE and ONFALSE used to process or not blocks of requirements and questions depending on the response given to the most previous Indicator will be specified by means of the annotation property @espd:groupVisibilityDependencyType (as shown below)</t>
-    </r>
-  </si>
-  <si>
-    <t>CRITERION_REQUIREMENT_SUBGROUP</t>
-  </si>
-  <si>
-    <t>@espd:dataStructureType</t>
-  </si>
-  <si>
-    <t>EVIDENCE</t>
-  </si>
-  <si>
-    <t>@espd:procssingIntstructionNote</t>
-  </si>
-  <si>
-    <t>Annotations (marked as @[AnnotationXXXXX] are subclasses of Processing Instructions used by software processors to know how to process an element (in this case a data element). Thus annotations can be used to warn a processor reading a criterion about the type of data structure, so the processor knows what algorithms to apply to this particular instance of data structure. See for example the annotation about the Evidence data structure, at the end of this example</t>
+    <t>@espd:processingIntstructionNote</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -485,11 +457,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -504,6 +471,19 @@
       <b/>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -908,7 +888,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1001,111 +981,114 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hipervínculo" xfId="42"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1121,7 +1104,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1408,30 +1391,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja10"/>
-  <dimension ref="A1:Z86"/>
+  <dimension ref="A1:Y86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="3.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="2" customWidth="1"/>
-    <col min="20" max="23" width="11.42578125" style="2" customWidth="1"/>
-    <col min="24" max="25" width="11.42578125" style="15" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="3.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.73046875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="3.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.3984375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="12.73046875" style="2" customWidth="1"/>
+    <col min="20" max="23" width="11.3984375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="23.265625" style="15" customWidth="1"/>
+    <col min="25" max="25" width="11.46484375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="11.3984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="24">
         <v>1</v>
       </c>
@@ -1492,7 +1473,7 @@
       <c r="T1" s="24">
         <v>20</v>
       </c>
-      <c r="U1" s="38">
+      <c r="U1" s="34">
         <v>21</v>
       </c>
       <c r="V1" s="24">
@@ -1507,31 +1488,28 @@
       <c r="Y1" s="24">
         <v>25</v>
       </c>
-      <c r="Z1" s="24">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:25" s="27" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
@@ -1562,34 +1540,31 @@
         <v>5</v>
       </c>
       <c r="X2" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z2" s="28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="29">
         <v>25</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
@@ -1602,138 +1577,130 @@
       <c r="P3" s="30"/>
       <c r="Q3" s="30"/>
       <c r="R3" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="30" t="s">
         <v>45</v>
-      </c>
-      <c r="S3" s="30" t="s">
-        <v>46</v>
       </c>
       <c r="T3" s="31"/>
       <c r="U3" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V3" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W3" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="X3" s="30" t="s">
-        <v>48</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="X3" s="30"/>
       <c r="Y3" s="30"/>
-      <c r="Z3" s="30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="29"/>
       <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="S4" s="42"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52"/>
-      <c r="X4" s="52"/>
-      <c r="Y4" s="52"/>
-      <c r="Z4" s="52"/>
-    </row>
-    <row r="5" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S4" s="35"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="45"/>
+    </row>
+    <row r="5" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="29"/>
       <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="S5" s="42"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="52"/>
-      <c r="Z5" s="52"/>
-    </row>
-    <row r="6" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="S5" s="35"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="45"/>
+      <c r="X5" s="45"/>
+      <c r="Y5" s="45"/>
+    </row>
+    <row r="6" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="29"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="S6" s="42"/>
-      <c r="T6" s="51"/>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="52"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="52"/>
-      <c r="Z6" s="52"/>
-    </row>
-    <row r="7" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="S6" s="35"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Y6" s="45"/>
+    </row>
+    <row r="7" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1750,43 +1717,40 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="T7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="T7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="U7" s="39" t="s">
+      <c r="V7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="W7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="V7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="X7" s="8" t="s">
+      <c r="X7" s="8"/>
+      <c r="Y7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1802,110 +1766,105 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="U8" s="6">
+        <v>8</v>
+      </c>
+      <c r="U8" s="8">
         <v>1</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="X8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="51" t="s">
         <v>73</v>
-      </c>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="50"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="50"/>
-      <c r="U9" s="50" t="s">
-        <v>76</v>
       </c>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
       <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="50"/>
-      <c r="T10" s="50"/>
-      <c r="U10" s="50" t="s">
-        <v>15</v>
+      <c r="E10" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="51" t="s">
+        <v>14</v>
       </c>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
       <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y10" s="6"/>
+    </row>
+    <row r="11" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1920,46 +1879,43 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="U11" s="8">
+        <v>1</v>
+      </c>
+      <c r="V11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="T11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="U11" s="6">
-        <v>1</v>
-      </c>
-      <c r="V11" s="6" t="s">
+      <c r="W11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="X11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1974,43 +1930,40 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="U12" s="8">
+        <v>1</v>
+      </c>
+      <c r="V12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="T12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="U12" s="6">
-        <v>1</v>
-      </c>
-      <c r="V12" s="6" t="s">
+      <c r="W12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="W12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="X12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -2026,40 +1979,37 @@
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="V13" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="X13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -2076,40 +2026,37 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="V14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="X14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -2129,27 +2076,24 @@
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
       <c r="U15" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V15" s="10"/>
       <c r="W15" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z15" s="10"/>
-    </row>
-    <row r="16" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="Y15" s="10"/>
+    </row>
+    <row r="16" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
@@ -2166,107 +2110,102 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="17"/>
       <c r="R16" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S16" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T16" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U16" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V16" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W16" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="X16" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y16" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z16" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="X16" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y16" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="17"/>
-      <c r="D17" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="48"/>
-      <c r="R17" s="48"/>
-      <c r="S17" s="48"/>
-      <c r="T17" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="U17" s="34"/>
-      <c r="V17" s="36"/>
+      <c r="D17" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="U17" s="52"/>
+      <c r="V17" s="33"/>
       <c r="W17" s="17"/>
       <c r="X17" s="18"/>
-      <c r="Y17" s="18"/>
-      <c r="Z17" s="17"/>
-    </row>
-    <row r="18" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y17" s="17"/>
+    </row>
+    <row r="18" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="17"/>
-      <c r="D18" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="48"/>
-      <c r="T18" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="U18" s="34"/>
-      <c r="V18" s="36"/>
+      <c r="D18" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="U18" s="52"/>
+      <c r="V18" s="33"/>
       <c r="W18" s="17"/>
       <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
-      <c r="Z18" s="17"/>
-    </row>
-    <row r="19" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y18" s="17"/>
+    </row>
+    <row r="19" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -2282,41 +2221,38 @@
       <c r="P19" s="17"/>
       <c r="Q19" s="17"/>
       <c r="R19" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S19" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="T19" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U19" s="18">
         <v>1</v>
       </c>
       <c r="V19" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="X19" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y19" s="18"/>
-      <c r="Z19" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
@@ -2332,39 +2268,36 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S20" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T20" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U20" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V20" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="W20" s="17"/>
-      <c r="X20" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y20" s="18"/>
-      <c r="Z20" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X20" s="18"/>
+      <c r="Y20" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
@@ -2380,110 +2313,103 @@
       <c r="P21" s="17"/>
       <c r="Q21" s="17"/>
       <c r="R21" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S21" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T21" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U21" s="18">
         <v>1</v>
       </c>
       <c r="V21" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W21" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="X21" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y21" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z21" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="5"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
-      <c r="E22" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="48"/>
-      <c r="P22" s="48"/>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="48"/>
-      <c r="S22" s="48"/>
-      <c r="T22" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="U22" s="36"/>
-      <c r="V22" s="36"/>
+      <c r="E22" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="U22" s="53"/>
+      <c r="V22" s="33"/>
       <c r="W22" s="17"/>
       <c r="X22" s="18"/>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="17"/>
-    </row>
-    <row r="23" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y22" s="17"/>
+    </row>
+    <row r="23" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
-      <c r="E23" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="48"/>
-      <c r="S23" s="48"/>
-      <c r="T23" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="U23" s="36"/>
-      <c r="V23" s="36"/>
+      <c r="E23" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="U23" s="53"/>
+      <c r="V23" s="33"/>
       <c r="W23" s="17"/>
       <c r="X23" s="18"/>
-      <c r="Y23" s="18"/>
-      <c r="Z23" s="17"/>
-    </row>
-    <row r="24" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y23" s="17"/>
+    </row>
+    <row r="24" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -2498,42 +2424,39 @@
       <c r="P24" s="17"/>
       <c r="Q24" s="17"/>
       <c r="R24" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S24" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T24" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="U24" s="17">
+        <v>55</v>
+      </c>
+      <c r="U24" s="18">
         <v>1</v>
       </c>
       <c r="V24" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W24" s="17"/>
-      <c r="X24" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y24" s="18"/>
-      <c r="Z24" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X24" s="18"/>
+      <c r="Y24" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
@@ -2548,41 +2471,38 @@
       <c r="P25" s="17"/>
       <c r="Q25" s="17"/>
       <c r="R25" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S25" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="T25" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="U25" s="17">
+        <v>57</v>
+      </c>
+      <c r="U25" s="18">
         <v>1</v>
       </c>
       <c r="V25" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="W25" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="X25" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y25" s="18"/>
-      <c r="Z25" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X25" s="18"/>
+      <c r="Y25" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
@@ -2598,39 +2518,36 @@
       <c r="P26" s="17"/>
       <c r="Q26" s="17"/>
       <c r="R26" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S26" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T26" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="U26" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="U26" s="18" t="s">
+        <v>8</v>
       </c>
       <c r="V26" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W26" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="X26" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y26" s="18"/>
-      <c r="Z26" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -2646,108 +2563,101 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S27" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U27" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="X27" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y27" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z27" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="5"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
-      <c r="E28" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="U28" s="9"/>
+      <c r="E28" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="38"/>
+      <c r="S28" s="38"/>
+      <c r="T28" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="U28" s="12"/>
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
       <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
-      <c r="Z28" s="9"/>
-    </row>
-    <row r="29" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="U29" s="9"/>
+      <c r="E29" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="T29" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="U29" s="12"/>
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
       <c r="X29" s="9"/>
       <c r="Y29" s="9"/>
-      <c r="Z29" s="9"/>
-    </row>
-    <row r="30" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2762,42 +2672,39 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U30" s="12">
         <v>1</v>
       </c>
       <c r="V30" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X30" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y30" s="12"/>
-      <c r="Z30" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -2812,111 +2719,104 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U31" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W31" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="X31" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y31" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z31" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="5"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="45"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="U32" s="9"/>
+      <c r="F32" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38"/>
+      <c r="R32" s="38"/>
+      <c r="S32" s="38"/>
+      <c r="T32" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="U32" s="12"/>
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
       <c r="X32" s="9"/>
       <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-    </row>
-    <row r="33" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="5"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="U33" s="9"/>
+      <c r="F33" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="38"/>
+      <c r="S33" s="38"/>
+      <c r="T33" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="U33" s="12"/>
       <c r="V33" s="9"/>
       <c r="W33" s="9"/>
       <c r="X33" s="9"/>
       <c r="Y33" s="9"/>
-      <c r="Z33" s="9"/>
-    </row>
-    <row r="34" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
       <c r="B34" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -2930,38 +2830,37 @@
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S34" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U34" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V34" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W34" s="5"/>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="12"/>
-      <c r="Z34" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X34" s="12"/>
+      <c r="Y34" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
       <c r="B35" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -2976,42 +2875,39 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S35" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U35" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V35" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W35" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X35" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y35" s="12"/>
-      <c r="Z35" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X35" s="12"/>
+      <c r="Y35" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
       <c r="B36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -3026,111 +2922,104 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U36" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="X36" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y36" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z36" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1"/>
       <c r="B37" s="5"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
-      <c r="T37" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="U37" s="9"/>
+      <c r="F37" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="38"/>
+      <c r="R37" s="38"/>
+      <c r="S37" s="38"/>
+      <c r="T37" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="U37" s="12"/>
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
       <c r="X37" s="9"/>
       <c r="Y37" s="9"/>
-      <c r="Z37" s="9"/>
-    </row>
-    <row r="38" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
       <c r="B38" s="5"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="45"/>
-      <c r="R38" s="45"/>
-      <c r="S38" s="45"/>
-      <c r="T38" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="U38" s="9"/>
+      <c r="F38" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="38"/>
+      <c r="N38" s="38"/>
+      <c r="O38" s="38"/>
+      <c r="P38" s="38"/>
+      <c r="Q38" s="38"/>
+      <c r="R38" s="38"/>
+      <c r="S38" s="38"/>
+      <c r="T38" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="U38" s="12"/>
       <c r="V38" s="9"/>
       <c r="W38" s="9"/>
       <c r="X38" s="9"/>
       <c r="Y38" s="9"/>
-      <c r="Z38" s="9"/>
-    </row>
-    <row r="39" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
       <c r="B39" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
@@ -3144,38 +3033,37 @@
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S39" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="T39" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U39" s="12">
         <v>1</v>
       </c>
       <c r="V39" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W39" s="5"/>
       <c r="X39" s="12"/>
-      <c r="Y39" s="12"/>
-      <c r="Z39" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y39" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
       <c r="B40" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -3190,42 +3078,39 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S40" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U40" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V40" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X40" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y40" s="12"/>
-      <c r="Z40" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X40" s="12"/>
+      <c r="Y40" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
@@ -3240,139 +3125,133 @@
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S41" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T41" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U41" s="12">
         <v>1</v>
       </c>
       <c r="V41" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W41" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="X41" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y41" s="21"/>
-      <c r="Z41" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="45"/>
-      <c r="R42" s="45"/>
-      <c r="S42" s="45"/>
-      <c r="T42" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="U42" s="45"/>
-      <c r="V42" s="45"/>
-      <c r="W42" s="45"/>
-      <c r="X42" s="45"/>
-      <c r="Y42" s="45"/>
-      <c r="Z42" s="45"/>
-    </row>
-    <row r="43" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="43"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="45"/>
-      <c r="M43" s="45"/>
-      <c r="N43" s="45"/>
-      <c r="O43" s="45"/>
-      <c r="P43" s="45"/>
-      <c r="Q43" s="45"/>
-      <c r="R43" s="45"/>
-      <c r="S43" s="45"/>
-      <c r="T43" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="U43" s="45"/>
-      <c r="V43" s="45"/>
-      <c r="W43" s="45"/>
-      <c r="X43" s="45"/>
-      <c r="Y43" s="45"/>
-      <c r="Z43" s="45"/>
-    </row>
-    <row r="44" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="45"/>
-      <c r="M44" s="45"/>
-      <c r="N44" s="45"/>
-      <c r="O44" s="45"/>
-      <c r="P44" s="45"/>
-      <c r="Q44" s="45"/>
-      <c r="R44" s="45"/>
-      <c r="S44" s="45"/>
-      <c r="T44" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="U44" s="45"/>
-      <c r="V44" s="45"/>
-      <c r="W44" s="45"/>
-      <c r="X44" s="45"/>
-      <c r="Y44" s="45"/>
-      <c r="Z44" s="45"/>
-    </row>
-    <row r="45" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
+      <c r="K42" s="38"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="38"/>
+      <c r="N42" s="38"/>
+      <c r="O42" s="38"/>
+      <c r="P42" s="38"/>
+      <c r="Q42" s="38"/>
+      <c r="R42" s="38"/>
+      <c r="S42" s="38"/>
+      <c r="T42" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="U42" s="54"/>
+      <c r="V42" s="38"/>
+      <c r="W42" s="38"/>
+      <c r="X42" s="38"/>
+      <c r="Y42" s="38"/>
+    </row>
+    <row r="43" spans="1:25" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+      <c r="S43" s="38"/>
+      <c r="T43" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="U43" s="54"/>
+      <c r="V43" s="38"/>
+      <c r="W43" s="38"/>
+      <c r="X43" s="38"/>
+      <c r="Y43" s="38"/>
+    </row>
+    <row r="44" spans="1:25" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="36"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="38"/>
+      <c r="S44" s="38"/>
+      <c r="T44" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="U44" s="54"/>
+      <c r="V44" s="38"/>
+      <c r="W44" s="38"/>
+      <c r="X44" s="38"/>
+      <c r="Y44" s="38"/>
+    </row>
+    <row r="45" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -3386,39 +3265,38 @@
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S45" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T45" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U45" s="12">
         <v>1</v>
       </c>
       <c r="V45" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W45" s="23"/>
       <c r="X45" s="12"/>
-      <c r="Y45" s="12"/>
-      <c r="Z45" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y45" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
@@ -3432,112 +3310,105 @@
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S46" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U46" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V46" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W46" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="X46" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y46" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z46" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="45"/>
-      <c r="O47" s="45"/>
-      <c r="P47" s="45"/>
-      <c r="Q47" s="45"/>
-      <c r="R47" s="45"/>
-      <c r="S47" s="45"/>
-      <c r="T47" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="U47" s="45"/>
-      <c r="V47" s="45"/>
-      <c r="W47" s="45"/>
-      <c r="X47" s="45"/>
-      <c r="Y47" s="45"/>
-      <c r="Z47" s="45"/>
-    </row>
-    <row r="48" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="43"/>
-      <c r="B48" s="44"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="H48" s="45"/>
-      <c r="I48" s="45"/>
-      <c r="J48" s="45"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="45"/>
-      <c r="M48" s="45"/>
-      <c r="N48" s="45"/>
-      <c r="O48" s="45"/>
-      <c r="P48" s="45"/>
-      <c r="Q48" s="45"/>
-      <c r="R48" s="45"/>
-      <c r="S48" s="45"/>
-      <c r="T48" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="U48" s="45"/>
-      <c r="V48" s="45"/>
-      <c r="W48" s="45"/>
-      <c r="X48" s="45"/>
-      <c r="Y48" s="45"/>
-      <c r="Z48" s="45"/>
-    </row>
-    <row r="49" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="X46" s="32"/>
+      <c r="Y46" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="36"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="38"/>
+      <c r="N47" s="38"/>
+      <c r="O47" s="38"/>
+      <c r="P47" s="38"/>
+      <c r="Q47" s="38"/>
+      <c r="R47" s="38"/>
+      <c r="S47" s="38"/>
+      <c r="T47" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="U47" s="54"/>
+      <c r="V47" s="38"/>
+      <c r="W47" s="38"/>
+      <c r="X47" s="38"/>
+      <c r="Y47" s="38"/>
+    </row>
+    <row r="48" spans="1:25" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="36"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="38"/>
+      <c r="O48" s="38"/>
+      <c r="P48" s="38"/>
+      <c r="Q48" s="38"/>
+      <c r="R48" s="38"/>
+      <c r="S48" s="38"/>
+      <c r="T48" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="U48" s="54"/>
+      <c r="V48" s="38"/>
+      <c r="W48" s="38"/>
+      <c r="X48" s="38"/>
+      <c r="Y48" s="38"/>
+    </row>
+    <row r="49" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
       <c r="B49" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -3550,41 +3421,38 @@
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
       <c r="R49" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S49" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T49" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="U49" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V49" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W49" s="13"/>
-      <c r="X49" s="35"/>
-      <c r="Y49" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z49" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X49" s="21"/>
+      <c r="Y49" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
@@ -3598,42 +3466,39 @@
       <c r="P50" s="5"/>
       <c r="Q50" s="5"/>
       <c r="R50" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S50" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U50" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="U50" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="V50" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X50" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y50" s="12"/>
-      <c r="Z50" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X50" s="12"/>
+      <c r="Y50" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
@@ -3648,39 +3513,36 @@
       <c r="P51" s="5"/>
       <c r="Q51" s="5"/>
       <c r="R51" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S51" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U51" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V51" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X51" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y51" s="12"/>
-      <c r="Z51" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X51" s="12"/>
+      <c r="Y51" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -3696,38 +3558,35 @@
       <c r="P52" s="5"/>
       <c r="Q52" s="5"/>
       <c r="R52" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S52" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T52" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U52" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V52" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W52" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X52" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y52" s="12"/>
-      <c r="Z52" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X52" s="12"/>
+      <c r="Y52" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
@@ -3744,46 +3603,43 @@
       <c r="P53" s="17"/>
       <c r="Q53" s="17"/>
       <c r="R53" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S53" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T53" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U53" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V53" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W53" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="X53" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y53" s="18"/>
-      <c r="Z53" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="X53" s="18"/>
+      <c r="Y53" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -3796,63 +3652,60 @@
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T54" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U54" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V54" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X54" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y54" s="4"/>
-      <c r="Z54" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>8</v>
+      </c>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="56" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="57" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="58" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="59" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="60" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="61" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="62" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="63" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="64" spans="1:25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="T49" r:id="rId1" display="EVIDENCE-00001"/>

</xml_diff>